<commit_message>
added tab for investments
</commit_message>
<xml_diff>
--- a/Tournament tracking/Tracking.xlsx
+++ b/Tournament tracking/Tracking.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
+    <sheet name="Investments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Person</t>
   </si>
@@ -63,12 +64,18 @@
   </si>
   <si>
     <t>Payout</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,4 +507,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>